<commit_message>
Balance Sheets modified. All Data sources work.
</commit_message>
<xml_diff>
--- a/home/BalanceSheet-Annual.xlsx
+++ b/home/BalanceSheet-Annual.xlsx
@@ -20,9 +20,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2005-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-Q1</t>
   </si>
   <si>
     <t xml:space="preserve">A.CURRENT ACCOUNT(Million USD)</t>
@@ -366,7 +420,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -378,7 +432,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1200" spc="140" strike="noStrike">
+              <a:defRPr b="1" sz="1200" spc="131" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="808080"/>
                 </a:solidFill>
@@ -386,7 +440,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1200" spc="140" strike="noStrike">
+              <a:rPr b="1" sz="1200" spc="131" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="808080"/>
                 </a:solidFill>
@@ -466,58 +520,58 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2002</c:v>
+                  <c:v>2002-Q1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2003</c:v>
+                  <c:v>2003-Q1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2004</c:v>
+                  <c:v>2004-Q1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2005</c:v>
+                  <c:v>2005-Q1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2006</c:v>
+                  <c:v>2006-Q1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2007</c:v>
+                  <c:v>2007-Q1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2008</c:v>
+                  <c:v>2008-Q1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2009</c:v>
+                  <c:v>2009-Q1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2010</c:v>
+                  <c:v>2010-Q1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2011</c:v>
+                  <c:v>2011-Q1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2012</c:v>
+                  <c:v>2012-Q1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2013</c:v>
+                  <c:v>2013-Q1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2014</c:v>
+                  <c:v>2014-Q1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015</c:v>
+                  <c:v>2015-Q1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016</c:v>
+                  <c:v>2016-Q1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2017</c:v>
+                  <c:v>2017-Q1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2018</c:v>
+                  <c:v>2018-Q1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2019</c:v>
+                  <c:v>2019-Q1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -595,11 +649,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="12181551"/>
-        <c:axId val="70314201"/>
+        <c:axId val="36602004"/>
+        <c:axId val="16668930"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="12181551"/>
+        <c:axId val="36602004"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,14 +695,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70314201"/>
+        <c:crossAx val="16668930"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70314201"/>
+        <c:axId val="16668930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -690,7 +744,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12181551"/>
+        <c:crossAx val="36602004"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -718,7 +772,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -730,7 +784,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1200" spc="140" strike="noStrike">
+              <a:defRPr b="1" sz="1200" spc="131" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="953735"/>
                 </a:solidFill>
@@ -738,7 +792,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1200" spc="140" strike="noStrike">
+              <a:rPr b="1" sz="1200" spc="131" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="953735"/>
                 </a:solidFill>
@@ -818,58 +872,58 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2002</c:v>
+                  <c:v>2002-Q1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2003</c:v>
+                  <c:v>2003-Q1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2004</c:v>
+                  <c:v>2004-Q1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2005</c:v>
+                  <c:v>2005-Q1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2006</c:v>
+                  <c:v>2006-Q1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2007</c:v>
+                  <c:v>2007-Q1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2008</c:v>
+                  <c:v>2008-Q1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2009</c:v>
+                  <c:v>2009-Q1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2010</c:v>
+                  <c:v>2010-Q1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2011</c:v>
+                  <c:v>2011-Q1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2012</c:v>
+                  <c:v>2012-Q1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2013</c:v>
+                  <c:v>2013-Q1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2014</c:v>
+                  <c:v>2014-Q1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015</c:v>
+                  <c:v>2015-Q1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016</c:v>
+                  <c:v>2016-Q1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2017</c:v>
+                  <c:v>2017-Q1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2018</c:v>
+                  <c:v>2018-Q1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2019</c:v>
+                  <c:v>2019-Q1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -995,58 +1049,58 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2002</c:v>
+                  <c:v>2002-Q1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2003</c:v>
+                  <c:v>2003-Q1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2004</c:v>
+                  <c:v>2004-Q1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2005</c:v>
+                  <c:v>2005-Q1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2006</c:v>
+                  <c:v>2006-Q1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2007</c:v>
+                  <c:v>2007-Q1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2008</c:v>
+                  <c:v>2008-Q1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2009</c:v>
+                  <c:v>2009-Q1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2010</c:v>
+                  <c:v>2010-Q1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2011</c:v>
+                  <c:v>2011-Q1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2012</c:v>
+                  <c:v>2012-Q1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2013</c:v>
+                  <c:v>2013-Q1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2014</c:v>
+                  <c:v>2014-Q1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015</c:v>
+                  <c:v>2015-Q1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016</c:v>
+                  <c:v>2016-Q1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2017</c:v>
+                  <c:v>2017-Q1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2018</c:v>
+                  <c:v>2018-Q1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2019</c:v>
+                  <c:v>2019-Q1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1124,11 +1178,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="96484378"/>
-        <c:axId val="18511039"/>
+        <c:axId val="7726493"/>
+        <c:axId val="35737049"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96484378"/>
+        <c:axId val="7726493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,14 +1224,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18511039"/>
+        <c:crossAx val="35737049"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18511039"/>
+        <c:axId val="35737049"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1273,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96484378"/>
+        <c:crossAx val="7726493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1271,7 +1325,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1371,58 +1425,58 @@
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2002</c:v>
+                  <c:v>2002-Q1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2003</c:v>
+                  <c:v>2003-Q1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2004</c:v>
+                  <c:v>2004-Q1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2005</c:v>
+                  <c:v>2005-Q1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2006</c:v>
+                  <c:v>2006-Q1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2007</c:v>
+                  <c:v>2007-Q1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2008</c:v>
+                  <c:v>2008-Q1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2009</c:v>
+                  <c:v>2009-Q1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2010</c:v>
+                  <c:v>2010-Q1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2011</c:v>
+                  <c:v>2011-Q1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2012</c:v>
+                  <c:v>2012-Q1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2013</c:v>
+                  <c:v>2013-Q1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2014</c:v>
+                  <c:v>2014-Q1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2015</c:v>
+                  <c:v>2015-Q1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2016</c:v>
+                  <c:v>2016-Q1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2017</c:v>
+                  <c:v>2017-Q1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2018</c:v>
+                  <c:v>2018-Q1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2019</c:v>
+                  <c:v>2019-Q1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1500,11 +1554,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6226574"/>
-        <c:axId val="83230770"/>
+        <c:axId val="19327965"/>
+        <c:axId val="5258027"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6226574"/>
+        <c:axId val="19327965"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,14 +1590,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83230770"/>
+        <c:crossAx val="5258027"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83230770"/>
+        <c:axId val="5258027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6226574"/>
+        <c:crossAx val="19327965"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1617,13 +1671,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>657000</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>510480</xdr:colOff>
+      <xdr:colOff>509400</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1631,8 +1685,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16660080" y="12138480"/>
-        <a:ext cx="5142960" cy="2767320"/>
+        <a:off x="13275000" y="12138840"/>
+        <a:ext cx="5141880" cy="2766240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1651,9 +1705,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>41400</xdr:colOff>
+      <xdr:colOff>40320</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1661,8 +1715,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9283680" y="12488760"/>
-        <a:ext cx="5249520" cy="2766960"/>
+        <a:off x="5898600" y="12488760"/>
+        <a:ext cx="5248440" cy="2765880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1681,9 +1735,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>128160</xdr:colOff>
+      <xdr:colOff>127080</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1691,8 +1745,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9632160" y="15783840"/>
-        <a:ext cx="4987800" cy="2766960"/>
+        <a:off x="6247080" y="15783840"/>
+        <a:ext cx="4986720" cy="2765880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1712,15 +1766,16 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="68.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="68.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.28"/>
@@ -1732,64 +1787,67 @@
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>2002</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2003</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>2005</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>2006</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>2007</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>2008</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>2009</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>2010</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2011</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>2013</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>2014</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>2015</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>2016</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>2017</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>2018</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>2019</v>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>-626</v>
@@ -1847,8 +1905,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>40705</v>
@@ -1906,8 +1967,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>47109</v>
@@ -1965,8 +2029,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>-6404</v>
@@ -2024,8 +2091,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>14045</v>
@@ -2083,8 +2153,11 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>6146</v>
@@ -2142,8 +2215,11 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>1495</v>
@@ -2201,8 +2277,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>2486</v>
@@ -2260,8 +2339,11 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>7040</v>
@@ -2320,10 +2402,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>-3059</v>
@@ -2382,10 +2464,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>2433</v>
@@ -2444,10 +2526,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0</v>
@@ -2506,10 +2588,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>-1172</v>
@@ -2568,10 +2650,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>143</v>
@@ -2630,10 +2712,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1082</v>
@@ -2692,10 +2774,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>2054</v>
@@ -2754,10 +2836,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1503</v>
@@ -2816,10 +2898,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>-16</v>
@@ -2878,10 +2960,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1519</v>
@@ -2940,10 +3022,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>819</v>
@@ -3002,10 +3084,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>30</v>
@@ -3064,10 +3146,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>42</v>
@@ -3126,10 +3208,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>-643</v>
@@ -3188,10 +3270,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>1390</v>
@@ -3250,10 +3332,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1603</v>
@@ -3312,10 +3394,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>1336</v>
@@ -3374,10 +3456,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>-669</v>
@@ -3436,10 +3518,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>-2016</v>
@@ -3498,10 +3580,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>2952</v>
@@ -3560,10 +3642,10 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>546</v>
@@ -3622,10 +3704,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>-758</v>
@@ -3684,10 +3766,10 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>212</v>
@@ -3746,10 +3828,10 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>-212</v>
@@ -3808,10 +3890,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>6153</v>
@@ -3870,10 +3952,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>-6365</v>
@@ -3932,10 +4014,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>0</v>

</xml_diff>